<commit_message>
Minor Infor test script update
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/testdata.xlsx
+++ b/src/main/resources/testdata/testdata.xlsx
@@ -1,31 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jazxz\Documents\SPI\SPI - ZN\Employment - ZN\Automation\Selenium Grid 2023 VSC - GIT\selenium-grid-docker\src\main\resources\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="login"/>
-    <sheet r:id="rId2" sheetId="2" name="testcases"/>
+    <sheet name="login" sheetId="1" r:id="rId1"/>
+    <sheet name="testcases" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>Test case name</t>
   </si>
   <si>
-    <t>UserName</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
     <t>TC1_Login</t>
   </si>
   <si>
@@ -69,17 +68,93 @@
   </si>
   <si>
     <t>Nav</t>
+  </si>
+  <si>
+    <t>infor_TC1_Login</t>
+  </si>
+  <si>
+    <t>infor_TC2_Registration</t>
+  </si>
+  <si>
+    <t>infor_TC3_LoginViaConfigFile</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>companyname</t>
+  </si>
+  <si>
+    <t>address1</t>
+  </si>
+  <si>
+    <t>address2</t>
+  </si>
+  <si>
+    <t>skill1</t>
+  </si>
+  <si>
+    <t>skill2</t>
+  </si>
+  <si>
+    <t>Zenric</t>
+  </si>
+  <si>
+    <t>Navea</t>
+  </si>
+  <si>
+    <t>jazx.zn@gmail.com</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>09661401029</t>
+  </si>
+  <si>
+    <t>RCG Technology Inc.</t>
+  </si>
+  <si>
+    <t>Address Line 1</t>
+  </si>
+  <si>
+    <t>Address Line 2</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>Selenium WebDriver</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -102,26 +177,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -132,10 +210,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -173,71 +251,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -265,7 +343,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -288,11 +366,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -301,13 +379,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -317,7 +395,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -326,7 +404,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -335,7 +413,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -343,10 +421,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -417,52 +495,52 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="9.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="9.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -475,62 +553,167 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="14.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="10.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="9.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="27.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L6" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F6" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added test for testing parallel execution
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/testdata.xlsx
+++ b/src/main/resources/testdata/testdata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
   <si>
     <t>Test case name</t>
   </si>
@@ -137,6 +137,15 @@
   </si>
   <si>
     <t>Selenium WebDriver</t>
+  </si>
+  <si>
+    <t>infor_TC1_Login2</t>
+  </si>
+  <si>
+    <t>infor_TC2_Registration2</t>
+  </si>
+  <si>
+    <t>infor_TC3_LoginViaConfigFile2</t>
   </si>
 </sst>
 </file>
@@ -553,10 +562,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,9 +719,73 @@
         <v>8</v>
       </c>
     </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J9" t="s">
+        <v>35</v>
+      </c>
+      <c r="K9" t="s">
+        <v>36</v>
+      </c>
+      <c r="L9" t="s">
+        <v>37</v>
+      </c>
+      <c r="M9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1"/>
+    <hyperlink ref="F9" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Additional test for parallel execution
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/testdata.xlsx
+++ b/src/main/resources/testdata/testdata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="48">
   <si>
     <t>Test case name</t>
   </si>
@@ -146,6 +146,24 @@
   </si>
   <si>
     <t>infor_TC3_LoginViaConfigFile2</t>
+  </si>
+  <si>
+    <t>infor_TC1_Login3</t>
+  </si>
+  <si>
+    <t>infor_TC2_Registration3</t>
+  </si>
+  <si>
+    <t>infor_TC3_LoginViaConfigFile3</t>
+  </si>
+  <si>
+    <t>infor_TC1_Login4</t>
+  </si>
+  <si>
+    <t>infor_TC2_Registration4</t>
+  </si>
+  <si>
+    <t>infor_TC3_LoginViaConfigFile4</t>
   </si>
 </sst>
 </file>
@@ -562,10 +580,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,10 +800,138 @@
         <v>8</v>
       </c>
     </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12" t="s">
+        <v>36</v>
+      </c>
+      <c r="L12" t="s">
+        <v>37</v>
+      </c>
+      <c r="M12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J15" t="s">
+        <v>35</v>
+      </c>
+      <c r="K15" t="s">
+        <v>36</v>
+      </c>
+      <c r="L15" t="s">
+        <v>37</v>
+      </c>
+      <c r="M15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1"/>
     <hyperlink ref="F9" r:id="rId2"/>
+    <hyperlink ref="F12" r:id="rId3"/>
+    <hyperlink ref="F15" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>